<commit_message>
Updates to tools features under new api design.
</commit_message>
<xml_diff>
--- a/tests/core/data/expected-integers.xlsx
+++ b/tests/core/data/expected-integers.xlsx
@@ -8,9 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IntegerModel" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="_step_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="_step_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="_step_3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="__footings__" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames/>
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,11 +36,6 @@
     <font>
       <name val="Calibri"/>
       <u val="single"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <i val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,25 +55,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
     <cellStyle name="bold" xfId="1" hidden="0"/>
     <cellStyle name="underline" xfId="2" hidden="0"/>
-    <cellStyle name="hyperlink" xfId="3" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -371,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C32"/>
+  <dimension ref="B2:C31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -404,7 +464,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IntegerModel(*, a, b, c) -&gt; 'IntegerModel'</t>
+          <t>IntegerModel(*, a: 'int', b: 'int', c: 'int', d: 'int') -&gt; 'IntegerModel'</t>
         </is>
       </c>
     </row>
@@ -414,180 +474,168 @@
           <t>Docstring:</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>The parent modeling class providing the key methods of run, audit, and visualize.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>a</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">    description for a</t>
+          <t>a : int</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>b</t>
+          <t xml:space="preserve">    A number A</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">    description for b</t>
+          <t>b : int</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>c</t>
+          <t xml:space="preserve">    A number B</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">    description for c</t>
+          <t>c : int</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number C</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>Steps</t>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>d : int</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>step_1</t>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number D</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Run step_1.</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>step_2</t>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>Assets</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Run step_2.</t>
+          <t>ret_1 : int</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="3" t="inlineStr">
-        <is>
-          <t>step_3</t>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Results a + b</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Run step_3.</t>
+          <t>ret_2 : int</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Results c - d</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>Methods</t>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ret_3 : int</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="C25" t="inlineStr">
         <is>
-          <t>run()</t>
+          <t xml:space="preserve">    Result total of step_1 and step_2</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="C26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Executes the model.</t>
-        </is>
-      </c>
+      <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>Steps</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Returns</t>
+          <t>1. _step_1 - Add a and b together.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">    int</t>
+          <t>2. _step_2 - Subtract d from c</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>3. _step_3 - Add total of steps 1 and 2.</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>audit(file, **kwargs)</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Creates an audit xlsx or json file.</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C21" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -598,7 +646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,7 +657,8 @@
     <col width="2.14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="1" customWidth="1" min="3" max="3"/>
-    <col width="1.2" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -621,7 +670,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
     </row>
@@ -629,96 +678,30 @@
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Signature:</t>
+          <t>Docstring:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>step_1(a, add)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5"/>
+          <t>Add a and b together.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr"/>
+    </row>
     <row r="6">
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Docstring:</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Run step_1.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>a : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>add : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Amount to add</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Returns</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="C17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="1" t="inlineStr">
-        <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ret_1</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>2</v>
       </c>
     </row>
@@ -733,7 +716,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -744,7 +727,8 @@
     <col width="2.14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="1" customWidth="1" min="3" max="3"/>
-    <col width="1.2" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -756,7 +740,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>_step_2</t>
         </is>
       </c>
     </row>
@@ -764,96 +748,30 @@
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Signature:</t>
+          <t>Docstring:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>step_2(b, subtract)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5"/>
+          <t>Subtract d from c</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr"/>
+    </row>
     <row r="6">
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Docstring:</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Run step_2.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>b : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>subtract : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Amount to subtract</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Returns</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="C17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="1" t="inlineStr">
-        <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ret_2</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -868,7 +786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,7 +797,8 @@
     <col width="2.14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="1" customWidth="1" min="3" max="3"/>
-    <col width="1.2" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -891,7 +810,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>_step_3</t>
         </is>
       </c>
     </row>
@@ -899,111 +818,31 @@
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Signature:</t>
+          <t>Docstring:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>step_3(a, b, c)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5"/>
+          <t>Add total of steps 1 and 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr"/>
+    </row>
     <row r="6">
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Docstring:</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Run step_3.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>a : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number A</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>b : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number B</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>c : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number C</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>Returns</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="C19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="1" t="inlineStr">
-        <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>3</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ret_3</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1017,7 +856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1809,7 +1648,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>IntegerModel</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1818,22 +1657,22 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1845,19 +1684,19 @@
         <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>2</v>
       </c>
       <c r="G34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1866,22 +1705,22 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1893,19 +1732,19 @@
         <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" t="n">
         <v>4</v>
       </c>
       <c r="G36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1914,13 +1753,13 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E37" t="n">
         <v>3</v>
       </c>
       <c r="F37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G37" t="n">
         <v>3</v>
@@ -1929,7 +1768,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1953,7 +1792,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1965,43 +1804,43 @@
         <v>6</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>6</v>
       </c>
       <c r="G39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G40" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2010,22 +1849,22 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2034,13 +1873,13 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E42" t="n">
         <v>3</v>
       </c>
       <c r="F42" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
         <v>3</v>
@@ -2049,7 +1888,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2058,22 +1897,22 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2082,13 +1921,13 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E44" t="n">
         <v>3</v>
       </c>
       <c r="F44" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G44" t="n">
         <v>3</v>
@@ -2097,7 +1936,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2106,13 +1945,13 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E45" t="n">
         <v>3</v>
       </c>
       <c r="F45" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G45" t="n">
         <v>3</v>
@@ -2121,7 +1960,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2130,22 +1969,22 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2154,46 +1993,46 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G47" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_2</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2202,22 +2041,22 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2226,13 +2065,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E50" t="n">
         <v>3</v>
       </c>
       <c r="F50" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G50" t="n">
         <v>3</v>
@@ -2241,7 +2080,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2250,13 +2089,13 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E51" t="n">
         <v>2</v>
       </c>
       <c r="F51" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G51" t="n">
         <v>2</v>
@@ -2265,31 +2104,31 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E52" t="n">
+        <v>3</v>
+      </c>
+      <c r="F52" t="n">
         <v>4</v>
       </c>
-      <c r="F52" t="n">
-        <v>18</v>
-      </c>
       <c r="G52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2298,22 +2137,22 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2322,22 +2161,22 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2346,904 +2185,40 @@
         </is>
       </c>
       <c r="D55" t="n">
+        <v>6</v>
+      </c>
+      <c r="E55" t="n">
         <v>4</v>
       </c>
-      <c r="E55" t="n">
-        <v>2</v>
-      </c>
       <c r="F55" t="n">
+        <v>6</v>
+      </c>
+      <c r="G55" t="n">
         <v>4</v>
-      </c>
-      <c r="G55" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>_step_3</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G56" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>6</v>
-      </c>
-      <c r="E57" t="n">
-        <v>2</v>
-      </c>
-      <c r="F57" t="n">
-        <v>6</v>
-      </c>
-      <c r="G57" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>6</v>
-      </c>
-      <c r="E58" t="n">
-        <v>3</v>
-      </c>
-      <c r="F58" t="n">
-        <v>6</v>
-      </c>
-      <c r="G58" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
-        <v>7</v>
-      </c>
-      <c r="E59" t="n">
-        <v>3</v>
-      </c>
-      <c r="F59" t="n">
-        <v>7</v>
-      </c>
-      <c r="G59" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>8</v>
-      </c>
-      <c r="E60" t="n">
-        <v>3</v>
-      </c>
-      <c r="F60" t="n">
-        <v>8</v>
-      </c>
-      <c r="G60" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>9</v>
-      </c>
-      <c r="E61" t="n">
-        <v>3</v>
-      </c>
-      <c r="F61" t="n">
-        <v>9</v>
-      </c>
-      <c r="G61" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>10</v>
-      </c>
-      <c r="E62" t="n">
-        <v>3</v>
-      </c>
-      <c r="F62" t="n">
-        <v>10</v>
-      </c>
-      <c r="G62" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>11</v>
-      </c>
-      <c r="E63" t="n">
-        <v>3</v>
-      </c>
-      <c r="F63" t="n">
-        <v>11</v>
-      </c>
-      <c r="G63" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>12</v>
-      </c>
-      <c r="E64" t="n">
-        <v>3</v>
-      </c>
-      <c r="F64" t="n">
-        <v>12</v>
-      </c>
-      <c r="G64" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D65" t="n">
-        <v>13</v>
-      </c>
-      <c r="E65" t="n">
-        <v>3</v>
-      </c>
-      <c r="F65" t="n">
-        <v>13</v>
-      </c>
-      <c r="G65" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>14</v>
-      </c>
-      <c r="E66" t="n">
-        <v>3</v>
-      </c>
-      <c r="F66" t="n">
-        <v>14</v>
-      </c>
-      <c r="G66" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>15</v>
-      </c>
-      <c r="E67" t="n">
-        <v>3</v>
-      </c>
-      <c r="F67" t="n">
-        <v>15</v>
-      </c>
-      <c r="G67" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>16</v>
-      </c>
-      <c r="E68" t="n">
-        <v>3</v>
-      </c>
-      <c r="F68" t="n">
-        <v>16</v>
-      </c>
-      <c r="G68" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>17</v>
-      </c>
-      <c r="E69" t="n">
-        <v>3</v>
-      </c>
-      <c r="F69" t="n">
-        <v>17</v>
-      </c>
-      <c r="G69" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>18</v>
-      </c>
-      <c r="E70" t="n">
-        <v>2</v>
-      </c>
-      <c r="F70" t="n">
-        <v>18</v>
-      </c>
-      <c r="G70" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>step_2</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>&lt;class 'int'&gt;</t>
-        </is>
-      </c>
-      <c r="D71" t="n">
-        <v>18</v>
-      </c>
-      <c r="E71" t="n">
-        <v>4</v>
-      </c>
-      <c r="F71" t="n">
-        <v>18</v>
-      </c>
-      <c r="G71" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D72" t="n">
-        <v>2</v>
-      </c>
-      <c r="E72" t="n">
-        <v>2</v>
-      </c>
-      <c r="F72" t="n">
-        <v>2</v>
-      </c>
-      <c r="G72" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D73" t="n">
-        <v>2</v>
-      </c>
-      <c r="E73" t="n">
-        <v>3</v>
-      </c>
-      <c r="F73" t="n">
-        <v>2</v>
-      </c>
-      <c r="G73" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D74" t="n">
-        <v>4</v>
-      </c>
-      <c r="E74" t="n">
-        <v>2</v>
-      </c>
-      <c r="F74" t="n">
-        <v>4</v>
-      </c>
-      <c r="G74" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D75" t="n">
-        <v>4</v>
-      </c>
-      <c r="E75" t="n">
-        <v>3</v>
-      </c>
-      <c r="F75" t="n">
-        <v>4</v>
-      </c>
-      <c r="G75" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D76" t="n">
-        <v>6</v>
-      </c>
-      <c r="E76" t="n">
-        <v>2</v>
-      </c>
-      <c r="F76" t="n">
-        <v>6</v>
-      </c>
-      <c r="G76" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D77" t="n">
-        <v>6</v>
-      </c>
-      <c r="E77" t="n">
-        <v>3</v>
-      </c>
-      <c r="F77" t="n">
-        <v>6</v>
-      </c>
-      <c r="G77" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D78" t="n">
-        <v>7</v>
-      </c>
-      <c r="E78" t="n">
-        <v>3</v>
-      </c>
-      <c r="F78" t="n">
-        <v>7</v>
-      </c>
-      <c r="G78" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D79" t="n">
-        <v>8</v>
-      </c>
-      <c r="E79" t="n">
-        <v>3</v>
-      </c>
-      <c r="F79" t="n">
-        <v>8</v>
-      </c>
-      <c r="G79" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D80" t="n">
-        <v>9</v>
-      </c>
-      <c r="E80" t="n">
-        <v>3</v>
-      </c>
-      <c r="F80" t="n">
-        <v>9</v>
-      </c>
-      <c r="G80" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>10</v>
-      </c>
-      <c r="E81" t="n">
-        <v>3</v>
-      </c>
-      <c r="F81" t="n">
-        <v>10</v>
-      </c>
-      <c r="G81" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D82" t="n">
-        <v>11</v>
-      </c>
-      <c r="E82" t="n">
-        <v>3</v>
-      </c>
-      <c r="F82" t="n">
-        <v>11</v>
-      </c>
-      <c r="G82" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D83" t="n">
-        <v>12</v>
-      </c>
-      <c r="E83" t="n">
-        <v>3</v>
-      </c>
-      <c r="F83" t="n">
-        <v>12</v>
-      </c>
-      <c r="G83" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D84" t="n">
-        <v>13</v>
-      </c>
-      <c r="E84" t="n">
-        <v>3</v>
-      </c>
-      <c r="F84" t="n">
-        <v>13</v>
-      </c>
-      <c r="G84" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D85" t="n">
-        <v>14</v>
-      </c>
-      <c r="E85" t="n">
-        <v>3</v>
-      </c>
-      <c r="F85" t="n">
-        <v>14</v>
-      </c>
-      <c r="G85" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D86" t="n">
-        <v>15</v>
-      </c>
-      <c r="E86" t="n">
-        <v>3</v>
-      </c>
-      <c r="F86" t="n">
-        <v>15</v>
-      </c>
-      <c r="G86" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D87" t="n">
-        <v>16</v>
-      </c>
-      <c r="E87" t="n">
-        <v>3</v>
-      </c>
-      <c r="F87" t="n">
-        <v>16</v>
-      </c>
-      <c r="G87" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D88" t="n">
-        <v>17</v>
-      </c>
-      <c r="E88" t="n">
-        <v>3</v>
-      </c>
-      <c r="F88" t="n">
-        <v>17</v>
-      </c>
-      <c r="G88" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D89" t="n">
-        <v>18</v>
-      </c>
-      <c r="E89" t="n">
-        <v>3</v>
-      </c>
-      <c r="F89" t="n">
-        <v>18</v>
-      </c>
-      <c r="G89" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>19</v>
-      </c>
-      <c r="E90" t="n">
-        <v>3</v>
-      </c>
-      <c r="F90" t="n">
-        <v>19</v>
-      </c>
-      <c r="G90" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>&lt;class 'str'&gt;</t>
-        </is>
-      </c>
-      <c r="D91" t="n">
-        <v>20</v>
-      </c>
-      <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="n">
-        <v>20</v>
-      </c>
-      <c r="G91" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>&lt;class 'int'&gt;</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>20</v>
-      </c>
-      <c r="E92" t="n">
-        <v>4</v>
-      </c>
-      <c r="F92" t="n">
-        <v>20</v>
-      </c>
-      <c r="G92" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>